<commit_message>
refactor(import): Refactor import programs and inventaries
</commit_message>
<xml_diff>
--- a/model-excel-import/courses.xlsx
+++ b/model-excel-import/courses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escuela Ingenieria\excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ei-sistema\model-excel-import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4A7C77-A94A-4395-8346-86714F67FB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9A976C-1F84-485F-8F75-8AE7667E6237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{87BA0F62-6263-4E3A-A9AA-29F1ED5A96B1}"/>
+    <workbookView xWindow="5430" yWindow="5295" windowWidth="15375" windowHeight="8415" xr2:uid="{87BA0F62-6263-4E3A-A9AA-29F1ED5A96B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>nombre</t>
   </si>
@@ -113,23 +113,16 @@
   </si>
   <si>
     <t>fecha_final</t>
+  </si>
+  <si>
+    <t>2024-04-20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-&quot;Bs&quot;* #,##0.00_-;\-&quot;Bs&quot;* #,##0.00_-;_-&quot;Bs&quot;* &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,17 +161,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -494,7 +484,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,11 +524,11 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2">
-        <v>45402</v>
-      </c>
-      <c r="E2" s="1">
-        <v>45342</v>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -551,11 +541,11 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1">
-        <v>45402</v>
-      </c>
-      <c r="E3" s="1">
-        <v>45828</v>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>